<commit_message>
Add new inventory workflow
Adds a workflow to implement new inventory creation including prompting the user for a file name and locations as well as which buildings to initialize the excel file with.

Implement Excel file creation and save functionality for new inventories.
</commit_message>
<xml_diff>
--- a/Campus/Kokomo.xlsx
+++ b/Campus/Kokomo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Local\College\24 Spring\SDEV220\Final Project\SDEV220-Project-Team-3\Campus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A23B87-EDB6-4D63-B7CB-307F41924480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3414A1F-DE45-4DA6-B393-5F5A322376BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="2100" windowWidth="34995" windowHeight="21705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-43980" yWindow="10665" windowWidth="34995" windowHeight="21705" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Building" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="148">
   <si>
     <t>Name</t>
   </si>
@@ -464,6 +464,9 @@
   </si>
   <si>
     <t>1976 Chevrolet Malibu</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
   </si>
 </sst>
 </file>
@@ -863,7 +866,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -890,7 +893,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>147</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>

</xml_diff>